<commit_message>
Implemented all clear and fixed a lot of issues, but still not updating in the stats menu/singleton
</commit_message>
<xml_diff>
--- a/ScoreSystem.xlsx
+++ b/ScoreSystem.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14920" tabRatio="500"/>
+    <workbookView xWindow="-100" yWindow="0" windowWidth="26280" windowHeight="14920" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,6 +16,14 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>Speed up too fast!</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -382,10 +390,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -445,7 +453,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B2:B15" si="4">(0.45/A3)+0.05</f>
+        <f t="shared" ref="B3:B15" si="4">(0.45/A3)+0.05</f>
         <v>0.2</v>
       </c>
       <c r="C3">
@@ -763,6 +771,11 @@
       <c r="G15">
         <f t="shared" si="3"/>
         <v>0.12666666666666668</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>